<commit_message>
Fixed model0, started model1
</commit_message>
<xml_diff>
--- a/supply_cap_demand_data.xlsx
+++ b/supply_cap_demand_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/l_martin_tue_nl/Documents/Transportation Teaching/1CM110/2023/Block 1/Solution/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas Henriquez\Documents\GitHub\Assignment-1-Decision-Making-in-Transport-and-Logistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="11_AD4DB114E441178AC67DF4DEAE53CB7E683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B5B612F-8EFC-48B2-AFA9-2469C07526F3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22350A2-EF23-4183-B575-7B598C9471B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-1965" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11250" yWindow="0" windowWidth="11250" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -419,9 +419,9 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +444,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -455,7 +455,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -466,7 +466,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -477,7 +477,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -488,7 +488,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -499,7 +499,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -516,7 +516,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -533,7 +533,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -550,7 +550,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -567,7 +567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Updated capacities for Model2
</commit_message>
<xml_diff>
--- a/supply_cap_demand_data.xlsx
+++ b/supply_cap_demand_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas Henriquez\Documents\GitHub\Assignment-1-Decision-Making-in-Transport-and-Logistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22350A2-EF23-4183-B575-7B598C9471B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF4169E-16F1-4819-99DF-38D6E382673E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11250" yWindow="0" windowWidth="11250" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -416,7 +416,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>